<commit_message>
add test of get_BQ to spreadsheet
</commit_message>
<xml_diff>
--- a/scripts/tests/test_by_hand.xlsx
+++ b/scripts/tests/test_by_hand.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason.debacker/repos/ProblemSet9/scripts/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F1FC13C-74D7-9E45-BF90-7D5B6B8E5400}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417AE3E9-3631-B04C-8E76-CF7F9AFACFC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="560" windowWidth="20620" windowHeight="12840" xr2:uid="{C29A7022-3D1E-4C46-A1B6-C7103E540419}"/>
+    <workbookView xWindow="43100" yWindow="460" windowWidth="30040" windowHeight="22640" xr2:uid="{C29A7022-3D1E-4C46-A1B6-C7103E540419}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FOCs" sheetId="1" r:id="rId1"/>
+    <sheet name="BQ" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>r, w, n_s, b_s, b_sp1</t>
   </si>
@@ -91,6 +92,12 @@
   </si>
   <si>
     <t>n_error</t>
+  </si>
+  <si>
+    <t>omega</t>
+  </si>
+  <si>
+    <t>g_n</t>
   </si>
 </sst>
 </file>
@@ -444,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCBD5A8-1DF7-354F-B895-AEACB91F65DB}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -508,7 +515,7 @@
         <v>0.4</v>
       </c>
       <c r="C7">
-        <v>0.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -534,7 +541,7 @@
       </c>
       <c r="C10">
         <f>(1+C3)*C6+C4*C5+C8-C7</f>
-        <v>0.67999999999999994</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -549,6 +556,9 @@
       <c r="B14">
         <v>0</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
@@ -557,6 +567,9 @@
       <c r="B15">
         <v>0.96</v>
       </c>
+      <c r="C15">
+        <v>0.96</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
@@ -565,8 +578,11 @@
       <c r="B16">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -574,63 +590,87 @@
         <f>B10^-B16</f>
         <v>1.7427485322789695</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <f>C10^-C16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="B19">
         <f>C10^-B16</f>
-        <v>2.1626297577854676</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>1</v>
+      </c>
+      <c r="C19" t="e">
+        <f>D10^-C16</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21">
         <f>B18 - B15*(1+C3)*(1-B14)*B19</f>
-        <v>-0.43718226356878187</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>0.73474853227896952</v>
+      </c>
+      <c r="C21" t="e">
+        <f>C18 - C15*(1+D3)*(1-C14)*C19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
       <c r="B25">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>18</v>
       </c>
       <c r="B26">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>19</v>
       </c>
       <c r="B27">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C27">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -638,14 +678,196 @@
         <f>((B26/B24)*((B5/B24)^(B27-1))*((1-((B5/B24)^B27))^((1-B27)/B27))) * B25</f>
         <v>0.20931219459067635</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C29">
+        <f>((C26/C24)*((C5/C24)^(C27-1))*((1-((C5/C24)^C27))^((1-C27)/C27))) * C25</f>
+        <v>0.20931219459067635</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>21</v>
       </c>
       <c r="B31">
         <f>B4*B18-B29</f>
         <v>1.8819860441440868</v>
+      </c>
+      <c r="C31">
+        <f>C4*C18-C29</f>
+        <v>0.99068780540932355</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A504245-574A-E04C-A3F8-DE0BE457F741}">
+  <dimension ref="A2:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0.4</v>
+      </c>
+      <c r="C2">
+        <v>0.4</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3">
+        <v>0.3</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.6</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <v>0.3</v>
+      </c>
+      <c r="D7">
+        <v>0.2</v>
+      </c>
+      <c r="F7">
+        <f>SUM(B7:D7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>0.3</v>
+      </c>
+      <c r="D8">
+        <v>0.2</v>
+      </c>
+      <c r="F8">
+        <f>SUM(B8:D8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="C9">
+        <f>B9*(C8/B8)</f>
+        <v>0.3</v>
+      </c>
+      <c r="D9">
+        <f>C9*(D8/C8)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F9">
+        <f>SUM(B9:D9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f>1-C7/B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="C11">
+        <f>1-(D7/C7)</f>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <f>((1+B13)/(1+B17))*(B7*B$11*B2+C2*C7*C$11+D2*D7*D$11)</f>
+        <v>0.12475247524752475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22">
+        <f>((1+B14)/(1+B18))*(B8*B$11*B3+C3*C8*C$11+D3*D8*D$11)</f>
+        <v>0.11215686274509802</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23">
+        <f>((1+B15)/(1+B19))*(B9*B$11*B4+C4*C9*C$11+D4*D9*D$11)</f>
+        <v>0.10098039215686273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>